<commit_message>
Added Links to Cost benefits Appraisl
</commit_message>
<xml_diff>
--- a/Estimation/Cost Benefit Appraisal.xlsx
+++ b/Estimation/Cost Benefit Appraisal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC26BC5-1C0B-4C87-B1F8-C5BCF6D15CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F28BCC-0AAF-40F7-994B-A941AE17E10D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7695" yWindow="2415" windowWidth="16770" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -95,16 +95,7 @@
     <t>Cumulative</t>
   </si>
   <si>
-    <t>2026 (Year 2) estimate inflation is 2.6%. 2027 (Year 3) estimate inflation is 2.1%. 2028 (Year 4) estimate inflation is 2.0%. 2029 (Year 5) estimate inflation is 2.9%</t>
-  </si>
-  <si>
     <t>Capital (Cloud Hosting)</t>
-  </si>
-  <si>
-    <t>£670/year (£0.002233 per request x estimated monthly requests)</t>
-  </si>
-  <si>
-    <t>One-Off Cloud Hosting payment of £1200</t>
   </si>
   <si>
     <t>Current (Transport API)</t>
@@ -133,6 +124,15 @@
   </si>
   <si>
     <t>Reduced boarding times could allow SYB to save annualy due to less overtime/fuel spent</t>
+  </si>
+  <si>
+    <t>£670/year (£0.002233 per request x estimated monthly requests) https://www.transportapi.com/pdf/TransportAPI-SASL-2022-customer-v4-selfserveplans.pdf</t>
+  </si>
+  <si>
+    <t>One-Off Cloud Hosting payment of £1200 (estimate) based on  https://www.spendflo.com/blog/digitalocean-pricing-guide</t>
+  </si>
+  <si>
+    <t>inflation based on https://www.in2013dollars.com/uk/inflation/2025?endYear=2030&amp;amount=100&amp;future_pct=0.03</t>
   </si>
 </sst>
 </file>
@@ -506,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,6 +558,9 @@
       <c r="F2" s="1"/>
       <c r="G2" s="3"/>
       <c r="H2" s="1"/>
+      <c r="I2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -591,7 +594,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -616,12 +619,12 @@
         <v>1200</v>
       </c>
       <c r="I4" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B5" s="4">
         <v>0</v>
@@ -633,28 +636,28 @@
         <v>1200</v>
       </c>
       <c r="E5" s="4">
-        <f>D5+(D5*0.21)</f>
-        <v>1452</v>
+        <f>D5+(D5*0.03)</f>
+        <v>1236</v>
       </c>
       <c r="F5" s="4">
-        <f t="shared" ref="F5:F7" si="0">E5+(E5*0.02)</f>
-        <v>1481.04</v>
+        <f>E5+(E5*0.03)</f>
+        <v>1273.08</v>
       </c>
       <c r="G5" s="4">
-        <f t="shared" ref="G5:G7" si="1">F5+(F5*0.029)</f>
-        <v>1523.9901600000001</v>
+        <f>F5+(F5*0.03)</f>
+        <v>1311.2723999999998</v>
       </c>
       <c r="H5" s="3">
-        <f t="shared" ref="H5:H6" si="2">SUM(B5:G5)</f>
-        <v>5657.0301600000003</v>
+        <f t="shared" ref="H5:H6" si="0">SUM(B5:G5)</f>
+        <v>5020.3523999999998</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="4">
         <v>0</v>
@@ -663,32 +666,32 @@
         <v>670</v>
       </c>
       <c r="D6" s="4">
-        <f t="shared" ref="D6:D7" si="3">C6+(C6*0.026)</f>
-        <v>687.42</v>
+        <f>C6+(C6*0.03)</f>
+        <v>690.1</v>
       </c>
       <c r="E6" s="4">
-        <f>D6+(D6*0.21)</f>
-        <v>831.77819999999997</v>
+        <f>D6+(D6*0.03)</f>
+        <v>710.803</v>
       </c>
       <c r="F6" s="4">
+        <f>E6+(E6*0.03)</f>
+        <v>732.12708999999995</v>
+      </c>
+      <c r="G6" s="4">
+        <f>F6+(F6*0.03)</f>
+        <v>754.0909026999999</v>
+      </c>
+      <c r="H6" s="3">
         <f t="shared" si="0"/>
-        <v>848.41376400000001</v>
-      </c>
-      <c r="G6" s="4">
-        <f t="shared" si="1"/>
-        <v>873.017763156</v>
-      </c>
-      <c r="H6" s="3">
-        <f t="shared" si="2"/>
-        <v>3910.6297271559997</v>
+        <v>3557.1209926999995</v>
       </c>
       <c r="I6" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B7" s="4">
         <v>0</v>
@@ -697,27 +700,27 @@
         <v>2000</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" si="3"/>
-        <v>2052</v>
+        <f>C7+(C7*0.03)</f>
+        <v>2060</v>
       </c>
       <c r="E7" s="4">
-        <f>D7+(D7*0.21)</f>
-        <v>2482.92</v>
+        <f>D7+(D7*0.03)</f>
+        <v>2121.8000000000002</v>
       </c>
       <c r="F7" s="4">
-        <f t="shared" si="0"/>
-        <v>2532.5783999999999</v>
+        <f>E7+(E7*0.03)</f>
+        <v>2185.4540000000002</v>
       </c>
       <c r="G7" s="4">
-        <f t="shared" si="1"/>
-        <v>2606.0231736000001</v>
+        <f>F7+(F7*0.03)</f>
+        <v>2251.0176200000001</v>
       </c>
       <c r="H7" s="3">
         <f>SUM(B7:G7)</f>
-        <v>11673.521573600001</v>
+        <v>10618.271620000001</v>
       </c>
       <c r="I7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -725,32 +728,32 @@
         <v>11</v>
       </c>
       <c r="B8" s="3">
-        <f>SUM(B3:B7)</f>
+        <f t="shared" ref="B8:G8" si="1">SUM(B3:B7)</f>
         <v>65000</v>
       </c>
       <c r="C8" s="3">
-        <f>SUM(C3:C7)</f>
+        <f t="shared" si="1"/>
         <v>3870</v>
       </c>
       <c r="D8" s="3">
-        <f>SUM(D3:D7)</f>
-        <v>3939.42</v>
+        <f t="shared" si="1"/>
+        <v>3950.1</v>
       </c>
       <c r="E8" s="3">
-        <f>SUM(E3:E7)</f>
-        <v>4766.6981999999998</v>
+        <f t="shared" si="1"/>
+        <v>4068.6030000000001</v>
       </c>
       <c r="F8" s="3">
-        <f>SUM(F3:F7)</f>
-        <v>4862.0321640000002</v>
+        <f t="shared" si="1"/>
+        <v>4190.6610899999996</v>
       </c>
       <c r="G8" s="3">
-        <f>SUM(G3:G7)</f>
-        <v>5003.0310967559999</v>
+        <f t="shared" si="1"/>
+        <v>4316.3809227000002</v>
       </c>
       <c r="H8" s="3">
         <f>SUM(H4:H7)</f>
-        <v>22441.181460756001</v>
+        <v>20395.745012700001</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -766,20 +769,20 @@
         <v>68870</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" ref="D9:G9" si="4">D8+C9</f>
-        <v>72809.42</v>
+        <f t="shared" ref="D9:G9" si="2">D8+C9</f>
+        <v>72820.100000000006</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" si="4"/>
-        <v>77576.118199999997</v>
+        <f t="shared" si="2"/>
+        <v>76888.703000000009</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="4"/>
-        <v>82438.150364000001</v>
+        <f t="shared" si="2"/>
+        <v>81079.364090000003</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="4"/>
-        <v>87441.181460755994</v>
+        <f t="shared" si="2"/>
+        <v>85395.745012700005</v>
       </c>
       <c r="H9" s="3"/>
     </row>
@@ -827,7 +830,7 @@
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B12" s="4">
         <v>0</v>
@@ -852,12 +855,12 @@
         <v>186480</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B13" s="4">
         <v>0</v>
@@ -878,11 +881,11 @@
         <v>2000</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" ref="H13" si="5">SUM(B13:G13)</f>
+        <f t="shared" ref="H13" si="3">SUM(B13:G13)</f>
         <v>10000</v>
       </c>
       <c r="I13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -890,31 +893,31 @@
         <v>11</v>
       </c>
       <c r="B14" s="3">
-        <f>SUM(B12:B13)</f>
+        <f t="shared" ref="B14:H14" si="4">SUM(B12:B13)</f>
         <v>0</v>
       </c>
       <c r="C14" s="3">
-        <f>SUM(C12:C13)</f>
+        <f t="shared" si="4"/>
         <v>38000</v>
       </c>
       <c r="D14" s="3">
-        <f>SUM(D12:D13)</f>
+        <f t="shared" si="4"/>
         <v>39620</v>
       </c>
       <c r="E14" s="3">
-        <f>SUM(E12:E13)</f>
+        <f t="shared" si="4"/>
         <v>39620</v>
       </c>
       <c r="F14" s="3">
-        <f>SUM(F12:F13)</f>
+        <f t="shared" si="4"/>
         <v>39620</v>
       </c>
       <c r="G14" s="3">
-        <f>SUM(G12:G13)</f>
+        <f t="shared" si="4"/>
         <v>39620</v>
       </c>
       <c r="H14" s="3">
-        <f>SUM(H12:H13)</f>
+        <f t="shared" si="4"/>
         <v>196480</v>
       </c>
     </row>
@@ -931,19 +934,19 @@
         <v>38000</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" ref="D15" si="6">D14+C15</f>
+        <f t="shared" ref="D15" si="5">D14+C15</f>
         <v>77620</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" ref="E15" si="7">E14+D15</f>
+        <f t="shared" ref="E15" si="6">E14+D15</f>
         <v>117240</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" ref="F15" si="8">F14+E15</f>
+        <f t="shared" ref="F15" si="7">F14+E15</f>
         <v>156860</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" ref="G15" si="9">G14+F15</f>
+        <f t="shared" ref="G15" si="8">G14+F15</f>
         <v>196480</v>
       </c>
       <c r="H15" s="3"/>
@@ -992,32 +995,32 @@
         <v>17</v>
       </c>
       <c r="B18" s="3">
-        <f>B14-B8</f>
+        <f t="shared" ref="B18:G18" si="9">B14-B8</f>
         <v>-65000</v>
       </c>
       <c r="C18" s="3">
-        <f>C14-C8</f>
+        <f t="shared" si="9"/>
         <v>34130</v>
       </c>
       <c r="D18" s="3">
-        <f>D14-D8</f>
-        <v>35680.58</v>
+        <f t="shared" si="9"/>
+        <v>35669.9</v>
       </c>
       <c r="E18" s="3">
-        <f>E14-E8</f>
-        <v>34853.301800000001</v>
+        <f t="shared" si="9"/>
+        <v>35551.396999999997</v>
       </c>
       <c r="F18" s="3">
-        <f>F14-F8</f>
-        <v>34757.967835999996</v>
+        <f t="shared" si="9"/>
+        <v>35429.338909999999</v>
       </c>
       <c r="G18" s="3">
-        <f>G14-G8</f>
-        <v>34616.968903244</v>
+        <f t="shared" si="9"/>
+        <v>35303.619077299998</v>
       </c>
       <c r="H18" s="3">
         <f>SUM(B18:G18)</f>
-        <v>109038.81853924401</v>
+        <v>111084.2549873</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1034,19 +1037,19 @@
       </c>
       <c r="D19" s="3">
         <f>D18+C19</f>
-        <v>4810.5800000000017</v>
+        <v>4799.9000000000015</v>
       </c>
       <c r="E19" s="3">
         <f>E18+D19</f>
-        <v>39663.881800000003</v>
+        <v>40351.296999999999</v>
       </c>
       <c r="F19" s="3">
         <f>F18+E19</f>
-        <v>74421.849635999999</v>
+        <v>75780.635909999997</v>
       </c>
       <c r="G19" s="3">
         <f t="shared" ref="G19" si="10">G18+F19</f>
-        <v>109038.81853924401</v>
+        <v>111084.2549873</v>
       </c>
       <c r="H19" s="3"/>
     </row>
@@ -1059,11 +1062,6 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>